<commit_message>
change url, add html
</commit_message>
<xml_diff>
--- a/teammember.xlsx
+++ b/teammember.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
   <si>
     <t>Imię</t>
   </si>
@@ -38,13 +38,34 @@
     <t>Drużyna</t>
   </si>
   <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>45gda</t>
+  </si>
+  <si>
+    <t>pawel@gmail.com</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>67GH</t>
+  </si>
+  <si>
+    <t>pawelr@gmail.com</t>
+  </si>
+  <si>
     <t>tes</t>
   </si>
   <si>
     <t>12dfa</t>
   </si>
   <si>
-    <t>test2</t>
+    <t>damian123@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -96,7 +117,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -108,8 +129,8 @@
     <col min="4" max="4" width="6.91015625" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="5.52734375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.9296875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="6.19921875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="8.4609375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="6.66796875" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="21.93359375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -160,28 +181,160 @@
       <c r="G2" t="s">
         <v>9</v>
       </c>
+      <c r="H2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
+      </c>
+      <c r="H3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>